<commit_message>
updated xls file for pmax hertz calculations
</commit_message>
<xml_diff>
--- a/mechanicalContact/hertzEquations/Pmax.xlsx
+++ b/mechanicalContact/hertzEquations/Pmax.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Fc (mN)</t>
   </si>
@@ -27,12 +27,15 @@
   <si>
     <t>Radius (µm)</t>
   </si>
+  <si>
+    <t>Fc (N)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +79,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -143,7 +153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,7 +174,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -259,53 +272,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$B$2:$B$77</c:f>
+              <c:f>'Contact de Hertz'!$C$2:$C$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>0.41064583501391122</c:v>
+                  <c:v>5.9908214249593286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51738133158568389</c:v>
+                  <c:v>7.5479620194674588</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70219450047675547</c:v>
+                  <c:v>10.244160537515866</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8847096322710799</c:v>
+                  <c:v>12.906833499718621</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.114664288743086</c:v>
+                  <c:v>16.261591213783802</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5128321909767322</c:v>
+                  <c:v>22.07037483227985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9060491223701663</c:v>
+                  <c:v>27.806929830259424</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4014714114078206</c:v>
+                  <c:v>35.034536226093508</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2592981524372107</c:v>
+                  <c:v>47.549181160670315</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1064583501391123</c:v>
+                  <c:v>59.908214249593286</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.1738133158568385</c:v>
+                  <c:v>75.479620194674567</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.8470963227108026</c:v>
+                  <c:v>129.06833499718624</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.146642887430858</c:v>
+                  <c:v>162.61591213783797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220.70374832279845</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>278.06929830259418</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350.34536226093519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -368,53 +399,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$C$2:$C$77</c:f>
+              <c:f>'Contact de Hertz'!$D$2:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>0.25869066579284195</c:v>
+                  <c:v>3.7739810097337294</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32592981524372122</c:v>
+                  <c:v>4.7549181160670342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4423548161355399</c:v>
+                  <c:v>6.4534167498593096</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5573321443715431</c:v>
+                  <c:v>8.1307956068919029</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.70219450047675547</c:v>
+                  <c:v>10.244160537515867</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95302456118508283</c:v>
+                  <c:v>13.903464915129709</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2007357057039107</c:v>
+                  <c:v>17.517268113046761</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5128321909767319</c:v>
+                  <c:v>22.07037483227985</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0532291750695553</c:v>
+                  <c:v>29.954107124796636</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5869066579284192</c:v>
+                  <c:v>37.739810097337291</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2592981524372115</c:v>
+                  <c:v>47.549181160670329</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5733214437154324</c:v>
+                  <c:v>81.307956068919054</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0219450047675531</c:v>
+                  <c:v>102.44160537515864</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>139.03464915129706</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>175.17268113046757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>220.70374832279859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,53 +526,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$D$2:$D$77</c:f>
+              <c:f>'Contact de Hertz'!$E$2:$E$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>0.16296490762186061</c:v>
+                  <c:v>2.3774590580335166</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20532291750695567</c:v>
+                  <c:v>2.9954107124796647</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27866607218577155</c:v>
+                  <c:v>4.0653978034459506</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35109725023837784</c:v>
+                  <c:v>5.1220802687579345</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44235481613553995</c:v>
+                  <c:v>6.4534167498593096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60036785285195526</c:v>
+                  <c:v>8.7586340565233769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75641609548836641</c:v>
+                  <c:v>11.03518741613993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.95302456118508294</c:v>
+                  <c:v>13.903464915129707</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2934533289642094</c:v>
+                  <c:v>18.869905048668638</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.629649076218606</c:v>
+                  <c:v>23.774590580335165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0532291750695562</c:v>
+                  <c:v>29.954107124796643</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5109725023837797</c:v>
+                  <c:v>51.220802687579358</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4235481613553986</c:v>
+                  <c:v>64.534167498593078</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87.586340565233755</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110.35187416139927</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>139.03464915129712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,53 +653,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$E$2:$E$77</c:f>
+              <c:f>'Contact de Hertz'!$F$2:$F$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>8.8470963227108013E-2</c:v>
+                  <c:v>1.2906833499718622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11146642887430865</c:v>
+                  <c:v>1.6261591213783806</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15128321909767325</c:v>
+                  <c:v>2.2070374832279853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19060491223701664</c:v>
+                  <c:v>2.7806929830259421</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.24014714114078212</c:v>
+                  <c:v>3.5034536226093511</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32592981524372122</c:v>
+                  <c:v>4.7549181160670333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.41064583501391139</c:v>
+                  <c:v>5.9908214249593312</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.51738133158568389</c:v>
+                  <c:v>7.547962019467457</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.70219450047675547</c:v>
+                  <c:v>10.244160537515864</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.88470963227108002</c:v>
+                  <c:v>12.906833499718619</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1146642887430862</c:v>
+                  <c:v>16.261591213783802</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9060491223701668</c:v>
+                  <c:v>27.806929830259431</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4014714114078206</c:v>
+                  <c:v>35.0345362260935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.549181160670322</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59.908214249593293</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75.479620194674595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,53 +780,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$F$2:$F$77</c:f>
+              <c:f>'Contact de Hertz'!$G$2:$G$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>5.5733214437154323E-2</c:v>
+                  <c:v>0.81307956068919029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0219450047675588E-2</c:v>
+                  <c:v>1.024416053751587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5302456118508308E-2</c:v>
+                  <c:v>1.3903464915129711</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1200735705703911</c:v>
+                  <c:v>1.751726811304676</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15128321909767325</c:v>
+                  <c:v>2.2070374832279853</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20532291750695564</c:v>
+                  <c:v>2.9954107124796647</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25869066579284211</c:v>
+                  <c:v>3.7739810097337303</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32592981524372122</c:v>
+                  <c:v>4.7549181160670333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4423548161355399</c:v>
+                  <c:v>6.4534167498593087</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.55733214437154321</c:v>
+                  <c:v>8.1307956068919029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.70219450047675569</c:v>
+                  <c:v>10.244160537515867</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2007357057039112</c:v>
+                  <c:v>17.517268113046764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5128321909767322</c:v>
+                  <c:v>22.07037483227985</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.954107124796639</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.739810097337291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47.549181160670351</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -804,53 +907,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$G$2:$G$77</c:f>
+              <c:f>'Contact de Hertz'!$H$2:$H$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>3.5109725023837773E-2</c:v>
+                  <c:v>0.51220802687579348</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4235481613553992E-2</c:v>
+                  <c:v>0.6453416749859312</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0036785285195508E-2</c:v>
+                  <c:v>0.87586340565233789</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5641609548836614E-2</c:v>
+                  <c:v>1.1035187416139929</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5302456118508266E-2</c:v>
+                  <c:v>1.3903464915129711</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12934533289642094</c:v>
+                  <c:v>1.8869905048668647</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16296490762186061</c:v>
+                  <c:v>2.3774590580335175</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.20532291750695555</c:v>
+                  <c:v>2.9954107124796647</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27866607218577139</c:v>
+                  <c:v>4.0653978034459506</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35109725023837773</c:v>
+                  <c:v>5.1220802687579345</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44235481613553984</c:v>
+                  <c:v>6.4534167498593105</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7564160954883663</c:v>
+                  <c:v>11.035187416139932</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.9530245611850825</c:v>
+                  <c:v>13.903464915129707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.869905048668642</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.774590580335172</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.954107124796657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,48 +1039,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$H$2:$H$14</c:f>
+              <c:f>'Contact de Hertz'!$I$2:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.906049122370166E-2</c:v>
+                  <c:v>0.27806929830259425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4014714114078212E-2</c:v>
+                  <c:v>0.35034536226093527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2592981524372115E-2</c:v>
+                  <c:v>0.4754918116067034</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1064583501391125E-2</c:v>
+                  <c:v>0.59908214249593306</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1738133158568386E-2</c:v>
+                  <c:v>0.7547962019467459</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0219450047675547E-2</c:v>
+                  <c:v>1.024416053751587</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.8470963227108013E-2</c:v>
+                  <c:v>1.2906833499718626</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1114664288743086</c:v>
+                  <c:v>1.6261591213783806</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.15128321909767317</c:v>
+                  <c:v>2.2070374832279849</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19060491223701656</c:v>
+                  <c:v>2.7806929830259421</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24014714114078206</c:v>
+                  <c:v>3.5034536226093516</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.41064583501391139</c:v>
+                  <c:v>5.9908214249593321</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.51738133158568378</c:v>
+                  <c:v>7.547962019467457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,11 +1095,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121110528"/>
-        <c:axId val="121111104"/>
+        <c:axId val="67135168"/>
+        <c:axId val="67139776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121110528"/>
+        <c:axId val="67135168"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1008,12 +1129,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121111104"/>
+        <c:crossAx val="67139776"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121111104"/>
+        <c:axId val="67139776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1044,7 +1165,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121110528"/>
+        <c:crossAx val="67135168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1142,53 +1263,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$B$2:$B$77</c:f>
+              <c:f>'Contact de Hertz'!$C$2:$C$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>0.41064583501391122</c:v>
+                  <c:v>5.9908214249593286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51738133158568389</c:v>
+                  <c:v>7.5479620194674588</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70219450047675547</c:v>
+                  <c:v>10.244160537515866</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8847096322710799</c:v>
+                  <c:v>12.906833499718621</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.114664288743086</c:v>
+                  <c:v>16.261591213783802</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5128321909767322</c:v>
+                  <c:v>22.07037483227985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9060491223701663</c:v>
+                  <c:v>27.806929830259424</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4014714114078206</c:v>
+                  <c:v>35.034536226093508</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2592981524372107</c:v>
+                  <c:v>47.549181160670315</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1064583501391123</c:v>
+                  <c:v>59.908214249593286</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.1738133158568385</c:v>
+                  <c:v>75.479620194674567</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.8470963227108026</c:v>
+                  <c:v>129.06833499718624</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.146642887430858</c:v>
+                  <c:v>162.61591213783797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220.70374832279845</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>278.06929830259418</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350.34536226093519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1251,53 +1390,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$C$2:$C$77</c:f>
+              <c:f>'Contact de Hertz'!$D$2:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>0.25869066579284195</c:v>
+                  <c:v>3.7739810097337294</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32592981524372122</c:v>
+                  <c:v>4.7549181160670342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4423548161355399</c:v>
+                  <c:v>6.4534167498593096</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5573321443715431</c:v>
+                  <c:v>8.1307956068919029</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.70219450047675547</c:v>
+                  <c:v>10.244160537515867</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95302456118508283</c:v>
+                  <c:v>13.903464915129709</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2007357057039107</c:v>
+                  <c:v>17.517268113046761</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5128321909767319</c:v>
+                  <c:v>22.07037483227985</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0532291750695553</c:v>
+                  <c:v>29.954107124796636</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5869066579284192</c:v>
+                  <c:v>37.739810097337291</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2592981524372115</c:v>
+                  <c:v>47.549181160670329</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5733214437154324</c:v>
+                  <c:v>81.307956068919054</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0219450047675531</c:v>
+                  <c:v>102.44160537515864</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>139.03464915129706</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>175.17268113046757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>220.70374832279859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,53 +1517,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$D$2:$D$77</c:f>
+              <c:f>'Contact de Hertz'!$E$2:$E$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>0.16296490762186061</c:v>
+                  <c:v>2.3774590580335166</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20532291750695567</c:v>
+                  <c:v>2.9954107124796647</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27866607218577155</c:v>
+                  <c:v>4.0653978034459506</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35109725023837784</c:v>
+                  <c:v>5.1220802687579345</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44235481613553995</c:v>
+                  <c:v>6.4534167498593096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60036785285195526</c:v>
+                  <c:v>8.7586340565233769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75641609548836641</c:v>
+                  <c:v>11.03518741613993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.95302456118508294</c:v>
+                  <c:v>13.903464915129707</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2934533289642094</c:v>
+                  <c:v>18.869905048668638</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.629649076218606</c:v>
+                  <c:v>23.774590580335165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0532291750695562</c:v>
+                  <c:v>29.954107124796643</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5109725023837797</c:v>
+                  <c:v>51.220802687579358</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4235481613553986</c:v>
+                  <c:v>64.534167498593078</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87.586340565233755</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110.35187416139927</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>139.03464915129712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1469,53 +1644,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$E$2:$E$77</c:f>
+              <c:f>'Contact de Hertz'!$F$2:$F$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>8.8470963227108013E-2</c:v>
+                  <c:v>1.2906833499718622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11146642887430865</c:v>
+                  <c:v>1.6261591213783806</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15128321909767325</c:v>
+                  <c:v>2.2070374832279853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19060491223701664</c:v>
+                  <c:v>2.7806929830259421</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.24014714114078212</c:v>
+                  <c:v>3.5034536226093511</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32592981524372122</c:v>
+                  <c:v>4.7549181160670333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.41064583501391139</c:v>
+                  <c:v>5.9908214249593312</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.51738133158568389</c:v>
+                  <c:v>7.547962019467457</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.70219450047675547</c:v>
+                  <c:v>10.244160537515864</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.88470963227108002</c:v>
+                  <c:v>12.906833499718619</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1146642887430862</c:v>
+                  <c:v>16.261591213783802</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9060491223701668</c:v>
+                  <c:v>27.806929830259431</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4014714114078206</c:v>
+                  <c:v>35.0345362260935</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.549181160670322</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59.908214249593293</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75.479620194674595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,53 +1771,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$F$2:$F$77</c:f>
+              <c:f>'Contact de Hertz'!$G$2:$G$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>5.5733214437154323E-2</c:v>
+                  <c:v>0.81307956068919029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0219450047675588E-2</c:v>
+                  <c:v>1.024416053751587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5302456118508308E-2</c:v>
+                  <c:v>1.3903464915129711</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1200735705703911</c:v>
+                  <c:v>1.751726811304676</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15128321909767325</c:v>
+                  <c:v>2.2070374832279853</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20532291750695564</c:v>
+                  <c:v>2.9954107124796647</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25869066579284211</c:v>
+                  <c:v>3.7739810097337303</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32592981524372122</c:v>
+                  <c:v>4.7549181160670333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4423548161355399</c:v>
+                  <c:v>6.4534167498593087</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.55733214437154321</c:v>
+                  <c:v>8.1307956068919029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.70219450047675569</c:v>
+                  <c:v>10.244160537515867</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2007357057039112</c:v>
+                  <c:v>17.517268113046764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5128321909767322</c:v>
+                  <c:v>22.07037483227985</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.954107124796639</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.739810097337291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47.549181160670351</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1687,53 +1898,71 @@
                 <c:pt idx="12">
                   <c:v>20000</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$G$2:$G$77</c:f>
+              <c:f>'Contact de Hertz'!$H$2:$H$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>3.5109725023837773E-2</c:v>
+                  <c:v>0.51220802687579348</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4235481613553992E-2</c:v>
+                  <c:v>0.6453416749859312</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0036785285195508E-2</c:v>
+                  <c:v>0.87586340565233789</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5641609548836614E-2</c:v>
+                  <c:v>1.1035187416139929</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5302456118508266E-2</c:v>
+                  <c:v>1.3903464915129711</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12934533289642094</c:v>
+                  <c:v>1.8869905048668647</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16296490762186061</c:v>
+                  <c:v>2.3774590580335175</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.20532291750695555</c:v>
+                  <c:v>2.9954107124796647</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27866607218577139</c:v>
+                  <c:v>4.0653978034459506</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35109725023837773</c:v>
+                  <c:v>5.1220802687579345</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44235481613553984</c:v>
+                  <c:v>6.4534167498593105</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7564160954883663</c:v>
+                  <c:v>11.035187416139932</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.9530245611850825</c:v>
+                  <c:v>13.903464915129707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.869905048668642</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.774590580335172</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.954107124796657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1801,48 +2030,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Contact de Hertz'!$H$2:$H$14</c:f>
+              <c:f>'Contact de Hertz'!$I$2:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.906049122370166E-2</c:v>
+                  <c:v>0.27806929830259425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4014714114078212E-2</c:v>
+                  <c:v>0.35034536226093527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2592981524372115E-2</c:v>
+                  <c:v>0.4754918116067034</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1064583501391125E-2</c:v>
+                  <c:v>0.59908214249593306</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1738133158568386E-2</c:v>
+                  <c:v>0.7547962019467459</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0219450047675547E-2</c:v>
+                  <c:v>1.024416053751587</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.8470963227108013E-2</c:v>
+                  <c:v>1.2906833499718626</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1114664288743086</c:v>
+                  <c:v>1.6261591213783806</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.15128321909767317</c:v>
+                  <c:v>2.2070374832279849</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19060491223701656</c:v>
+                  <c:v>2.7806929830259421</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24014714114078206</c:v>
+                  <c:v>3.5034536226093516</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.41064583501391139</c:v>
+                  <c:v>5.9908214249593321</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.51738133158568378</c:v>
+                  <c:v>7.547962019467457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1857,12 +2086,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121118016"/>
-        <c:axId val="71647232"/>
+        <c:axId val="173965888"/>
+        <c:axId val="173966464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121118016"/>
+        <c:axId val="173965888"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1890,13 +2120,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71647232"/>
+        <c:crossAx val="173966464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71647232"/>
+        <c:axId val="173966464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,7 +2156,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121118016"/>
+        <c:crossAx val="173965888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1952,13 +2182,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>349135</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>25631</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>195349</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>139239</xdr:rowOff>
@@ -1982,13 +2212,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
@@ -2032,13 +2262,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>403860</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
@@ -2097,13 +2327,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>220980</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
@@ -2162,13 +2392,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>2331720</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>563880</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>14548</xdr:rowOff>
@@ -2194,13 +2424,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>327660</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -2244,13 +2474,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>2766060</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
@@ -2309,13 +2539,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
@@ -2662,813 +2892,1032 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="5.77734375" style="1" customWidth="1"/>
-    <col min="5" max="8" width="5.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="2"/>
-    <col min="10" max="10" width="40.77734375" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="5.77734375" style="1" customWidth="1"/>
+    <col min="6" max="11" width="5.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="40.77734375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="J1" s="6" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="L1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <f t="shared" ref="B2:B14" si="0">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$5))^(2/3)</f>
-        <v>0.41064583501391122</v>
+        <f>A2*0.001</f>
+        <v>1E-3</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C12" si="1">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$6))^(2/3)</f>
-        <v>0.25869066579284195</v>
+        <f t="shared" ref="C2:C17" si="0">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$5))^(2/3)</f>
+        <v>5.9908214249593286</v>
       </c>
       <c r="D2" s="3">
-        <f>1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$7))^(2/3)</f>
-        <v>0.16296490762186061</v>
-      </c>
-      <c r="E2" s="3">
-        <f>1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$8))^(2/3)</f>
-        <v>8.8470963227108013E-2</v>
+        <f t="shared" ref="D2:D14" si="1">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$6))^(2/3)</f>
+        <v>3.7739810097337294</v>
+      </c>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E14" si="2">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$7))^(2/3)</f>
+        <v>2.3774590580335166</v>
       </c>
       <c r="F2" s="3">
-        <f>1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$9))^(2/3)</f>
-        <v>5.5733214437154323E-2</v>
-      </c>
-      <c r="G2" s="3">
-        <f>1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$10))^(2/3)</f>
-        <v>3.5109725023837773E-2</v>
-      </c>
-      <c r="H2" s="3">
-        <f>1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$11))^(2/3)</f>
-        <v>1.906049122370166E-2</v>
-      </c>
-      <c r="J2" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F2:F14" si="3">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$8))^(2/3)</f>
+        <v>1.2906833499718622</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G14" si="4">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$9))^(2/3)</f>
+        <v>0.81307956068919029</v>
+      </c>
+      <c r="H2" s="8">
+        <f t="shared" ref="H2:H14" si="5">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$10))^(2/3)</f>
+        <v>0.51220802687579348</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" ref="I2:I15" si="6">1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$11))^(2/3)</f>
+        <v>0.27806929830259425</v>
+      </c>
+      <c r="J2" s="3">
+        <f>1.5*((A2^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$12))^(2/3)</f>
+        <v>0.1103518741613993</v>
+      </c>
+      <c r="L2" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3">
+        <f t="shared" ref="B3:B17" si="7">A3*0.001</f>
+        <v>2E-3</v>
+      </c>
+      <c r="C3" s="3">
         <f t="shared" si="0"/>
-        <v>0.51738133158568389</v>
-      </c>
-      <c r="C3" s="3">
+        <v>7.5479620194674588</v>
+      </c>
+      <c r="D3" s="3">
         <f t="shared" si="1"/>
-        <v>0.32592981524372122</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D12" si="2">1.5*((A3^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$7))^(2/3)</f>
-        <v>0.20532291750695567</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E12" si="3">1.5*((A3^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$8))^(2/3)</f>
-        <v>0.11146642887430865</v>
+        <v>4.7549181160670342</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" si="2"/>
+        <v>2.9954107124796647</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F12" si="4">1.5*((A3^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$9))^(2/3)</f>
-        <v>7.0219450047675588E-2</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:H12" si="5">1.5*((A3^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$10))^(2/3)</f>
-        <v>4.4235481613553992E-2</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H14" si="6">1.5*((A3^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$11))^(2/3)</f>
-        <v>2.4014714114078212E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>1.6261591213783806</v>
+      </c>
+      <c r="G3" s="8">
+        <f t="shared" si="4"/>
+        <v>1.024416053751587</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" si="5"/>
+        <v>0.6453416749859312</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" si="6"/>
+        <v>0.35034536226093527</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J15" si="8">1.5*((A3^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$12))^(2/3)</f>
+        <v>0.13903464915129715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>5</v>
       </c>
       <c r="B4" s="3">
+        <f t="shared" si="7"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>0.70219450047675547</v>
-      </c>
-      <c r="C4" s="3">
+        <v>10.244160537515866</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" si="1"/>
-        <v>0.4423548161355399</v>
-      </c>
-      <c r="D4" s="3">
+        <v>6.4534167498593096</v>
+      </c>
+      <c r="E4" s="8">
         <f t="shared" si="2"/>
-        <v>0.27866607218577155</v>
-      </c>
-      <c r="E4" s="3">
+        <v>4.0653978034459506</v>
+      </c>
+      <c r="F4" s="3">
         <f t="shared" si="3"/>
-        <v>0.15128321909767325</v>
-      </c>
-      <c r="F4" s="3">
+        <v>2.2070374832279853</v>
+      </c>
+      <c r="G4" s="8">
         <f t="shared" si="4"/>
-        <v>9.5302456118508308E-2</v>
-      </c>
-      <c r="G4" s="3">
+        <v>1.3903464915129711</v>
+      </c>
+      <c r="H4" s="8">
         <f t="shared" si="5"/>
-        <v>6.0036785285195508E-2</v>
-      </c>
-      <c r="H4" s="3">
+        <v>0.87586340565233789</v>
+      </c>
+      <c r="I4" s="3">
         <f t="shared" si="6"/>
-        <v>3.2592981524372115E-2</v>
-      </c>
-      <c r="J4" s="6" t="s">
+        <v>0.4754918116067034</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="8"/>
+        <v>0.18869905048668648</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>10</v>
       </c>
       <c r="B5" s="3">
+        <f t="shared" si="7"/>
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>0.8847096322710799</v>
-      </c>
-      <c r="C5" s="3">
+        <v>12.906833499718621</v>
+      </c>
+      <c r="D5" s="3">
         <f t="shared" si="1"/>
-        <v>0.5573321443715431</v>
-      </c>
-      <c r="D5" s="3">
+        <v>8.1307956068919029</v>
+      </c>
+      <c r="E5" s="8">
         <f t="shared" si="2"/>
-        <v>0.35109725023837784</v>
-      </c>
-      <c r="E5" s="3">
+        <v>5.1220802687579345</v>
+      </c>
+      <c r="F5" s="3">
         <f t="shared" si="3"/>
-        <v>0.19060491223701664</v>
-      </c>
-      <c r="F5" s="3">
+        <v>2.7806929830259421</v>
+      </c>
+      <c r="G5" s="8">
         <f t="shared" si="4"/>
-        <v>0.1200735705703911</v>
-      </c>
-      <c r="G5" s="3">
+        <v>1.751726811304676</v>
+      </c>
+      <c r="H5" s="8">
         <f t="shared" si="5"/>
-        <v>7.5641609548836614E-2</v>
-      </c>
-      <c r="H5" s="3">
+        <v>1.1035187416139929</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="6"/>
-        <v>4.1064583501391125E-2</v>
-      </c>
-      <c r="J5" s="5">
+        <v>0.59908214249593306</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="8"/>
+        <v>0.23774590580335175</v>
+      </c>
+      <c r="L5" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>20</v>
       </c>
       <c r="B6" s="3">
+        <f t="shared" si="7"/>
+        <v>0.02</v>
+      </c>
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>1.114664288743086</v>
-      </c>
-      <c r="C6" s="3">
+        <v>16.261591213783802</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>0.70219450047675547</v>
-      </c>
-      <c r="D6" s="3">
+        <v>10.244160537515867</v>
+      </c>
+      <c r="E6" s="8">
         <f t="shared" si="2"/>
-        <v>0.44235481613553995</v>
-      </c>
-      <c r="E6" s="3">
+        <v>6.4534167498593096</v>
+      </c>
+      <c r="F6" s="3">
         <f t="shared" si="3"/>
-        <v>0.24014714114078212</v>
-      </c>
-      <c r="F6" s="3">
+        <v>3.5034536226093511</v>
+      </c>
+      <c r="G6" s="8">
         <f t="shared" si="4"/>
-        <v>0.15128321909767325</v>
-      </c>
-      <c r="G6" s="3">
+        <v>2.2070374832279853</v>
+      </c>
+      <c r="H6" s="8">
         <f t="shared" si="5"/>
-        <v>9.5302456118508266E-2</v>
-      </c>
-      <c r="H6" s="3">
+        <v>1.3903464915129711</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="6"/>
-        <v>5.1738133158568386E-2</v>
-      </c>
-      <c r="J6" s="5">
+        <v>0.7547962019467459</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="8"/>
+        <v>0.29954107124796653</v>
+      </c>
+      <c r="L6" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>50</v>
       </c>
       <c r="B7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>1.5128321909767322</v>
-      </c>
-      <c r="C7" s="3">
+        <v>22.07037483227985</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>0.95302456118508283</v>
-      </c>
-      <c r="D7" s="3">
+        <v>13.903464915129709</v>
+      </c>
+      <c r="E7" s="8">
         <f t="shared" si="2"/>
-        <v>0.60036785285195526</v>
-      </c>
-      <c r="E7" s="3">
+        <v>8.7586340565233769</v>
+      </c>
+      <c r="F7" s="3">
         <f t="shared" si="3"/>
-        <v>0.32592981524372122</v>
-      </c>
-      <c r="F7" s="3">
+        <v>4.7549181160670333</v>
+      </c>
+      <c r="G7" s="8">
         <f t="shared" si="4"/>
-        <v>0.20532291750695564</v>
-      </c>
-      <c r="G7" s="3">
+        <v>2.9954107124796647</v>
+      </c>
+      <c r="H7" s="8">
         <f t="shared" si="5"/>
-        <v>0.12934533289642094</v>
-      </c>
-      <c r="H7" s="3">
+        <v>1.8869905048668647</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="6"/>
-        <v>7.0219450047675547E-2</v>
-      </c>
-      <c r="J7" s="5">
+        <v>1.024416053751587</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="8"/>
+        <v>0.40653978034459515</v>
+      </c>
+      <c r="L7" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>100</v>
       </c>
       <c r="B8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>1.9060491223701663</v>
-      </c>
-      <c r="C8" s="3">
+        <v>27.806929830259424</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>1.2007357057039107</v>
-      </c>
-      <c r="D8" s="3">
+        <v>17.517268113046761</v>
+      </c>
+      <c r="E8" s="8">
         <f t="shared" si="2"/>
-        <v>0.75641609548836641</v>
-      </c>
-      <c r="E8" s="3">
+        <v>11.03518741613993</v>
+      </c>
+      <c r="F8" s="3">
         <f t="shared" si="3"/>
-        <v>0.41064583501391139</v>
-      </c>
-      <c r="F8" s="3">
+        <v>5.9908214249593312</v>
+      </c>
+      <c r="G8" s="8">
         <f t="shared" si="4"/>
-        <v>0.25869066579284211</v>
-      </c>
-      <c r="G8" s="3">
+        <v>3.7739810097337303</v>
+      </c>
+      <c r="H8" s="8">
         <f t="shared" si="5"/>
-        <v>0.16296490762186061</v>
-      </c>
-      <c r="H8" s="3">
+        <v>2.3774590580335175</v>
+      </c>
+      <c r="I8" s="3">
         <f t="shared" si="6"/>
-        <v>8.8470963227108013E-2</v>
-      </c>
-      <c r="J8" s="5">
+        <v>1.2906833499718626</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="8"/>
+        <v>0.5122080268757937</v>
+      </c>
+      <c r="L8" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>200</v>
       </c>
       <c r="B9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>2.4014714114078206</v>
-      </c>
-      <c r="C9" s="3">
+        <v>35.034536226093508</v>
+      </c>
+      <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>1.5128321909767319</v>
-      </c>
-      <c r="D9" s="3">
+        <v>22.07037483227985</v>
+      </c>
+      <c r="E9" s="8">
         <f t="shared" si="2"/>
-        <v>0.95302456118508294</v>
-      </c>
-      <c r="E9" s="3">
+        <v>13.903464915129707</v>
+      </c>
+      <c r="F9" s="3">
         <f t="shared" si="3"/>
-        <v>0.51738133158568389</v>
-      </c>
-      <c r="F9" s="3">
+        <v>7.547962019467457</v>
+      </c>
+      <c r="G9" s="8">
         <f t="shared" si="4"/>
-        <v>0.32592981524372122</v>
-      </c>
-      <c r="G9" s="3">
+        <v>4.7549181160670333</v>
+      </c>
+      <c r="H9" s="8">
         <f t="shared" si="5"/>
-        <v>0.20532291750695555</v>
-      </c>
-      <c r="H9" s="3">
+        <v>2.9954107124796647</v>
+      </c>
+      <c r="I9" s="3">
         <f t="shared" si="6"/>
-        <v>0.1114664288743086</v>
-      </c>
-      <c r="J9" s="5">
+        <v>1.6261591213783806</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="8"/>
+        <v>0.64534167498593109</v>
+      </c>
+      <c r="L9" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>500</v>
       </c>
       <c r="B10" s="3">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>3.2592981524372107</v>
-      </c>
-      <c r="C10" s="3">
+        <v>47.549181160670315</v>
+      </c>
+      <c r="D10" s="3">
         <f t="shared" si="1"/>
-        <v>2.0532291750695553</v>
-      </c>
-      <c r="D10" s="3">
+        <v>29.954107124796636</v>
+      </c>
+      <c r="E10" s="8">
         <f t="shared" si="2"/>
-        <v>1.2934533289642094</v>
-      </c>
-      <c r="E10" s="3">
+        <v>18.869905048668638</v>
+      </c>
+      <c r="F10" s="3">
         <f t="shared" si="3"/>
-        <v>0.70219450047675547</v>
-      </c>
-      <c r="F10" s="3">
+        <v>10.244160537515864</v>
+      </c>
+      <c r="G10" s="8">
         <f t="shared" si="4"/>
-        <v>0.4423548161355399</v>
-      </c>
-      <c r="G10" s="3">
+        <v>6.4534167498593087</v>
+      </c>
+      <c r="H10" s="8">
         <f t="shared" si="5"/>
-        <v>0.27866607218577139</v>
-      </c>
-      <c r="H10" s="3">
+        <v>4.0653978034459506</v>
+      </c>
+      <c r="I10" s="3">
         <f t="shared" si="6"/>
-        <v>0.15128321909767317</v>
-      </c>
-      <c r="J10" s="5">
+        <v>2.2070374832279849</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="8"/>
+        <v>0.87586340565233778</v>
+      </c>
+      <c r="L10" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1000</v>
       </c>
       <c r="B11" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>4.1064583501391123</v>
-      </c>
-      <c r="C11" s="3">
+        <v>59.908214249593286</v>
+      </c>
+      <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>2.5869066579284192</v>
-      </c>
-      <c r="D11" s="3">
+        <v>37.739810097337291</v>
+      </c>
+      <c r="E11" s="8">
         <f t="shared" si="2"/>
-        <v>1.629649076218606</v>
-      </c>
-      <c r="E11" s="3">
+        <v>23.774590580335165</v>
+      </c>
+      <c r="F11" s="3">
         <f t="shared" si="3"/>
-        <v>0.88470963227108002</v>
-      </c>
-      <c r="F11" s="3">
+        <v>12.906833499718619</v>
+      </c>
+      <c r="G11" s="8">
         <f t="shared" si="4"/>
-        <v>0.55733214437154321</v>
-      </c>
-      <c r="G11" s="3">
+        <v>8.1307956068919029</v>
+      </c>
+      <c r="H11" s="8">
         <f t="shared" si="5"/>
-        <v>0.35109725023837773</v>
-      </c>
-      <c r="H11" s="3">
+        <v>5.1220802687579345</v>
+      </c>
+      <c r="I11" s="3">
         <f t="shared" si="6"/>
-        <v>0.19060491223701656</v>
-      </c>
-      <c r="J11" s="5">
+        <v>2.7806929830259421</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="8"/>
+        <v>1.1035187416139929</v>
+      </c>
+      <c r="L11" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2000</v>
       </c>
       <c r="B12" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>5.1738133158568385</v>
-      </c>
-      <c r="C12" s="3">
+        <v>75.479620194674567</v>
+      </c>
+      <c r="D12" s="3">
         <f t="shared" si="1"/>
-        <v>3.2592981524372115</v>
-      </c>
-      <c r="D12" s="3">
+        <v>47.549181160670329</v>
+      </c>
+      <c r="E12" s="8">
         <f t="shared" si="2"/>
-        <v>2.0532291750695562</v>
-      </c>
-      <c r="E12" s="3">
+        <v>29.954107124796643</v>
+      </c>
+      <c r="F12" s="3">
         <f t="shared" si="3"/>
-        <v>1.1146642887430862</v>
-      </c>
-      <c r="F12" s="3">
+        <v>16.261591213783802</v>
+      </c>
+      <c r="G12" s="8">
         <f t="shared" si="4"/>
-        <v>0.70219450047675569</v>
-      </c>
-      <c r="G12" s="3">
+        <v>10.244160537515867</v>
+      </c>
+      <c r="H12" s="8">
         <f t="shared" si="5"/>
-        <v>0.44235481613553984</v>
-      </c>
-      <c r="H12" s="3">
+        <v>6.4534167498593105</v>
+      </c>
+      <c r="I12" s="3">
         <f t="shared" si="6"/>
-        <v>0.24014714114078206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.5034536226093516</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="8"/>
+        <v>1.3903464915129711</v>
+      </c>
+      <c r="L12" s="5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10000</v>
       </c>
       <c r="B13" s="3">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>8.8470963227108026</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" ref="C13" si="7">1.5*((A13^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$6))^(2/3)</f>
-        <v>5.5733214437154324</v>
+        <v>129.06833499718624</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13" si="8">1.5*((A13^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$7))^(2/3)</f>
-        <v>3.5109725023837797</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" ref="E13" si="9">1.5*((A13^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$8))^(2/3)</f>
-        <v>1.9060491223701668</v>
+        <f t="shared" si="1"/>
+        <v>81.307956068919054</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="2"/>
+        <v>51.220802687579358</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" ref="F13" si="10">1.5*((A13^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$9))^(2/3)</f>
-        <v>1.2007357057039112</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" ref="G13:H13" si="11">1.5*((A13^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$10))^(2/3)</f>
-        <v>0.7564160954883663</v>
-      </c>
-      <c r="H13" s="3">
+        <f t="shared" si="3"/>
+        <v>27.806929830259431</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="4"/>
+        <v>17.517268113046764</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="5"/>
+        <v>11.035187416139932</v>
+      </c>
+      <c r="I13" s="3">
         <f t="shared" si="6"/>
-        <v>0.41064583501391139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.9908214249593321</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="8"/>
+        <v>2.3774590580335184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>20000</v>
       </c>
       <c r="B14" s="3">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>11.146642887430858</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" ref="C14" si="12">1.5*((A14^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$6))^(2/3)</f>
-        <v>7.0219450047675531</v>
+        <v>162.61591213783797</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" ref="D14" si="13">1.5*((A14^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$7))^(2/3)</f>
-        <v>4.4235481613553986</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" ref="E14" si="14">1.5*((A14^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$8))^(2/3)</f>
-        <v>2.4014714114078206</v>
+        <f t="shared" si="1"/>
+        <v>102.44160537515864</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="2"/>
+        <v>64.534167498593078</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" ref="F14" si="15">1.5*((A14^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$9))^(2/3)</f>
-        <v>1.5128321909767322</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" ref="G14:H14" si="16">1.5*((A14^(1/3))/PI())*((4*((1/1000)+(1/3))^(-1))/(3*$J$10))^(2/3)</f>
-        <v>0.9530245611850825</v>
-      </c>
-      <c r="H14" s="3">
+        <f t="shared" si="3"/>
+        <v>35.0345362260935</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="4"/>
+        <v>22.07037483227985</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="5"/>
+        <v>13.903464915129707</v>
+      </c>
+      <c r="I14" s="3">
         <f t="shared" si="6"/>
-        <v>0.51738133158568378</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+        <v>7.547962019467457</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="8"/>
+        <v>2.9954107124796643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>220.70374832279845</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ref="D15" si="9">1.5*((A15^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$6))^(2/3)</f>
+        <v>139.03464915129706</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" ref="E15" si="10">1.5*((A15^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$7))^(2/3)</f>
+        <v>87.586340565233755</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ref="F15" si="11">1.5*((A15^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$8))^(2/3)</f>
+        <v>47.549181160670322</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" ref="G15" si="12">1.5*((A15^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$9))^(2/3)</f>
+        <v>29.954107124796639</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" ref="H15" si="13">1.5*((A15^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$10))^(2/3)</f>
+        <v>18.869905048668642</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="6"/>
+        <v>10.244160537515867</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="8"/>
+        <v>4.0653978034459506</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>278.06929830259418</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16:D17" si="14">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$6))^(2/3)</f>
+        <v>175.17268113046757</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" ref="E16:E17" si="15">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$7))^(2/3)</f>
+        <v>110.35187416139927</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ref="F16:F17" si="16">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$8))^(2/3)</f>
+        <v>59.908214249593293</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" ref="G16:G17" si="17">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$9))^(2/3)</f>
+        <v>37.739810097337291</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" ref="H16:H17" si="18">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$10))^(2/3)</f>
+        <v>23.774590580335172</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:I17" si="19">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$11))^(2/3)</f>
+        <v>12.906833499718623</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" ref="J16:J17" si="20">1.5*((A16^(1/3))/PI())*((4*((1/1000)+(1/$L$2))^(-1))/(3*$L$12))^(2/3)</f>
+        <v>5.1220802687579354</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>200000</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>350.34536226093519</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="14"/>
+        <v>220.70374832279859</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="15"/>
+        <v>139.03464915129712</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="16"/>
+        <v>75.479620194674595</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="17"/>
+        <v>47.549181160670351</v>
+      </c>
+      <c r="H17" s="8">
+        <f t="shared" si="18"/>
+        <v>29.954107124796657</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="19"/>
+        <v>16.261591213783809</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="20"/>
+        <v>6.4534167498593131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="2"/>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="2"/>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>